<commit_message>
decent working version.Better functionalities to be added-4th version
</commit_message>
<xml_diff>
--- a/PersonalTT/GCN.xlsx
+++ b/PersonalTT/GCN.xlsx
@@ -69,16 +69,16 @@
     <t>MON</t>
   </si>
   <si>
-    <t>WP</t>
-  </si>
-  <si>
-    <t>WP(B3)</t>
+    <t>WP(7)</t>
+  </si>
+  <si>
+    <t>WP(B3)(7)</t>
   </si>
   <si>
     <t>TUE</t>
   </si>
   <si>
-    <t>DSC(B2)</t>
+    <t>DSC(B2)(3)</t>
   </si>
   <si>
     <t>WED</t>
@@ -87,7 +87,7 @@
     <t>THU</t>
   </si>
   <si>
-    <t>WP(B1)</t>
+    <t>WP(B1)(7)</t>
   </si>
   <si>
     <t>FRI</t>
@@ -144,7 +144,7 @@
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border/>
     <border>
       <left style="medium">
@@ -173,20 +173,6 @@
         <color rgb="FF000000"/>
       </right>
       <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -288,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -301,11 +287,8 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -316,20 +299,20 @@
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -337,7 +320,13 @@
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -639,10 +628,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -714,103 +703,176 @@
       </c>
     </row>
     <row r="4" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A5" s="4" t="s">
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A7" s="16"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A8" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A9" s="16"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A11" s="16"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A8" s="4" t="s">
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A9" s="5" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A13" s="16"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A15" s="16"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -831,10 +893,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -906,85 +968,159 @@
       </c>
     </row>
     <row r="4" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A7" s="16"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A7" s="4" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A9" s="16"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A8" s="4" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A11" s="16"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" customHeight="1" ht="20.1">
-      <c r="A9" s="5" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A13" s="16"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" customHeight="1" ht="20.1">
+      <c r="A15" s="16"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>

</xml_diff>

<commit_message>
Last version.Will no longer be able to work on this
</commit_message>
<xml_diff>
--- a/PersonalTT/GCN.xlsx
+++ b/PersonalTT/GCN.xlsx
@@ -749,7 +749,9 @@
       <c r="A7" s="16"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -868,6 +870,7 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F11:G11"/>

</xml_diff>